<commit_message>
copied from KickJr Github repo
</commit_message>
<xml_diff>
--- a/Hardware/Basic/PPG-Module/NotSoSmartWatch-BASIC-PPG-MODULE-BOM.xlsx
+++ b/Hardware/Basic/PPG-Module/NotSoSmartWatch-BASIC-PPG-MODULE-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10615"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlandohoilett/Documents/Milestones/Git/Tasks-Tutorials-Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlandohoilett/Documents/Milestones/Git/KickJr/Hardware/Basic/PPG-Module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6F0319-899B-F545-ABC0-B856698FB7B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90A2DBB-F77C-524B-8B3A-09DC1A4CED05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="20020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,211 +225,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{4414EC97-401B-5C4D-BF38-03085F1F044A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{42ADFC76-2A16-3F4B-9937-20E1DF8DC9D9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{92578C3E-17AC-CF40-B33B-C67DBD723ACA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{B87F5F84-059E-824D-B1C3-C6D21A6C0FC3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{8D3ED184-945A-F444-9885-2E4FC0FBB6A7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{7F187FCD-1E21-9644-AE5D-0FA5E52F65FA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Orlando Hoilett:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This is just an example to show you what information to list and how to list them.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>BOM #</t>
   </si>
@@ -470,139 +271,103 @@
     <t>SMD</t>
   </si>
   <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Price per unit</t>
   </si>
   <si>
-    <t>10k resistor</t>
-  </si>
-  <si>
     <t>0603</t>
   </si>
   <si>
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t>Stackpole Electronics Inc</t>
-  </si>
-  <si>
-    <t>1uF capacitor</t>
-  </si>
-  <si>
-    <t>LM358</t>
-  </si>
-  <si>
-    <t>Photoresistor</t>
-  </si>
-  <si>
-    <t>9V Battery Connector</t>
-  </si>
-  <si>
-    <t>1µF ±10% 25V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>CL10A105KA8NNNC</t>
-  </si>
-  <si>
-    <t>1276-1102-1-ND</t>
-  </si>
-  <si>
     <t>Per 100</t>
   </si>
   <si>
-    <t>White  LED Indication - Discrete 2.9V Radial</t>
-  </si>
-  <si>
     <t>THT</t>
   </si>
   <si>
-    <t>Radial</t>
-  </si>
-  <si>
-    <t>American Bright Optoelectronics Corporation</t>
-  </si>
-  <si>
-    <t>BL-BZX3V4V-1-B02</t>
-  </si>
-  <si>
-    <t>BL-BZX3V4V-1-B02-ND</t>
-  </si>
-  <si>
-    <t>White LED</t>
-  </si>
-  <si>
-    <t>Battery Connector, Snap 9V 1 Cell Wire Leads - 4" (101.6mm)</t>
-  </si>
-  <si>
-    <t>Keystone Electronics</t>
-  </si>
-  <si>
-    <t>81-4</t>
-  </si>
-  <si>
-    <t>36-81-4-ND</t>
-  </si>
-  <si>
-    <t>9V</t>
-  </si>
-  <si>
     <t>LED1</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>General Purpose Amplifier 2 Circuit  8-SOIC</t>
-  </si>
-  <si>
-    <t>8-SOIC</t>
-  </si>
-  <si>
-    <t>LM358DR</t>
-  </si>
-  <si>
-    <t>296-1014-1-ND</t>
-  </si>
-  <si>
-    <t>OP1</t>
-  </si>
-  <si>
     <t>Total (in Bulk)</t>
   </si>
   <si>
-    <t>CDS Cell 520nm 27 ~ 60kOhms @ 10 lux</t>
-  </si>
-  <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>Advanced Photonix</t>
-  </si>
-  <si>
-    <t>PDV-P8104</t>
-  </si>
-  <si>
-    <t>PDV-P8104-ND</t>
-  </si>
-  <si>
-    <t>10 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
-  </si>
-  <si>
-    <t>R1,R2,R3</t>
-  </si>
-  <si>
-    <t>RMCF0603FT10K0</t>
-  </si>
-  <si>
-    <t>RMCF0603FT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>Design Name -- Revision Code / Designer or Organization Name</t>
+    <t>Kick Jr PPG Module Rev A / Purdue Milestones</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Green 525nm LED Indication - Discrete 3.1V 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>1516-1084-1-ND</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>QT Brightek (QTB)</t>
+  </si>
+  <si>
+    <t>QBLP631-IG</t>
+  </si>
+  <si>
+    <t>2.2µF ±10% 10V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>2.2µF capacitor</t>
+  </si>
+  <si>
+    <t>CL10A225KP8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1085-1-ND</t>
+  </si>
+  <si>
+    <t>Photodiode</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>Photodiode 940nm 100ns 130° 2-SMD, Gull Wing, PHOTODIODE PIN HI SPEED HI SENS</t>
+  </si>
+  <si>
+    <t>2-SMD, Gull Wing</t>
+  </si>
+  <si>
+    <t>Vishay Semiconductor Opto Division</t>
+  </si>
+  <si>
+    <t>VBPW34S</t>
+  </si>
+  <si>
+    <t>751-1500-1-ND</t>
+  </si>
+  <si>
+    <t>0.05' spaced Header Pins</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 50 position 0.050" (1.27mm)</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>GRPB501VWVN-RC</t>
+  </si>
+  <si>
+    <t>S9014E-50-ND</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -613,7 +378,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -682,13 +447,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -856,7 +614,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -893,6 +651,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1314,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -1339,7 +1106,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1352,18 +1119,18 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="6">
-        <f>SUM(M3:M77)</f>
-        <v>2.48</v>
+        <f>SUM(M3:M6)</f>
+        <v>4.79</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="O1" s="6">
-        <f>SUM(O3:O77)</f>
-        <v>1.1271</v>
+        <f>SUM(O3:O6)</f>
+        <v>3.2529000000000003</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
@@ -1398,312 +1165,215 @@
         <v>8</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="17" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
-        <f>1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>21</v>
+      <c r="B3" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>45</v>
+      <c r="J3" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="K3" s="10">
-        <v>0.38</v>
+        <v>1.19</v>
       </c>
       <c r="L3" s="11">
         <v>1</v>
       </c>
       <c r="M3" s="10">
-        <f t="shared" ref="M3:M8" si="0">K3*L3</f>
-        <v>0.38</v>
+        <f>K3*L3</f>
+        <v>1.19</v>
       </c>
       <c r="N3" s="10">
-        <v>0.1391</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="O3" s="10">
-        <f t="shared" ref="O3:O7" si="1">L3*N3</f>
-        <v>0.1391</v>
+        <f>N3*L3</f>
+        <v>0.56599999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="17" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="K4" s="10">
-        <v>0.89</v>
+        <v>0.39</v>
       </c>
       <c r="L4" s="11">
         <v>1</v>
       </c>
       <c r="M4" s="10">
-        <f t="shared" si="0"/>
-        <v>0.89</v>
+        <f t="shared" ref="M4:M6" si="0">K4*L4</f>
+        <v>0.39</v>
       </c>
       <c r="N4" s="10">
-        <v>0.46</v>
+        <v>0.16170000000000001</v>
       </c>
       <c r="O4" s="10">
-        <f t="shared" si="1"/>
-        <v>0.46</v>
+        <f t="shared" ref="O4:O6" si="1">N4*L4</f>
+        <v>0.16170000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" s="17" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G5" s="9" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="K5" s="10">
-        <v>0.55000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="L5" s="11">
         <v>1</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="N5" s="10">
-        <v>0.3982</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="O5" s="10">
         <f t="shared" si="1"/>
-        <v>0.3982</v>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" s="17" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="K6" s="10">
-        <v>0.26</v>
+        <v>3.11</v>
       </c>
       <c r="L6" s="11">
         <v>1</v>
       </c>
       <c r="M6" s="10">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>3.11</v>
       </c>
       <c r="N6" s="10">
-        <v>9.0899999999999995E-2</v>
+        <v>2.4912000000000001</v>
       </c>
       <c r="O6" s="10">
         <f t="shared" si="1"/>
-        <v>9.0899999999999995E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="L7" s="11">
-        <v>3</v>
-      </c>
-      <c r="M7" s="10">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="N7" s="10">
-        <v>6.7999999999999996E-3</v>
-      </c>
-      <c r="O7" s="10">
-        <f t="shared" si="1"/>
-        <v>2.0399999999999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="L8" s="11">
-        <v>1</v>
-      </c>
-      <c r="M8" s="10">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="N8" s="10">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="O8" s="10">
-        <f>L8*N8</f>
-        <v>1.8499999999999999E-2</v>
+        <v>2.4912000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>